<commit_message>
falta apropiar de acuerdo a glosas y listo
</commit_message>
<xml_diff>
--- a/data/parametros.xlsx
+++ b/data/parametros.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10950" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="clasificador" sheetId="1" r:id="rId1"/>
     <sheet name="movimientos" sheetId="2" r:id="rId2"/>
+    <sheet name="palabras" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="345">
   <si>
     <t>Nivel 2</t>
   </si>
@@ -840,9 +841,6 @@
     <t>Encaje Legal</t>
   </si>
   <si>
-    <t>Ver Glosa</t>
-  </si>
-  <si>
     <t>Ingreso</t>
   </si>
   <si>
@@ -880,13 +878,196 @@
   </si>
   <si>
     <t>Garantias-Empresas Públicas</t>
+  </si>
+  <si>
+    <t>ENVIBOL</t>
+  </si>
+  <si>
+    <t>Comibol</t>
+  </si>
+  <si>
+    <t>PalabrasClave</t>
+  </si>
+  <si>
+    <t>ENARSA</t>
+  </si>
+  <si>
+    <t>ENERGIA ARGENTINA</t>
+  </si>
+  <si>
+    <t>PETROLEO BRASILERO</t>
+  </si>
+  <si>
+    <t>TRAFIGURA</t>
+  </si>
+  <si>
+    <t>REFINOR</t>
+  </si>
+  <si>
+    <t>GAS TOTAL</t>
+  </si>
+  <si>
+    <t>MOVIMIENTO DEL FONDO RAL</t>
+  </si>
+  <si>
+    <t>CUENTAS DE ORGANISMOS INTERNACIONALES</t>
+  </si>
+  <si>
+    <t>PAGO POR RETRIBUCION AL TITULAR</t>
+  </si>
+  <si>
+    <t>DIESEL OIL</t>
+  </si>
+  <si>
+    <t>ENATEX</t>
+  </si>
+  <si>
+    <t>PAGO POR LA PLANILLA DE AVANCE</t>
+  </si>
+  <si>
+    <t>CONSORCIO MINERO</t>
+  </si>
+  <si>
+    <t>POR DESEMBOLSO</t>
+  </si>
+  <si>
+    <t>DEPOSITANTE</t>
+  </si>
+  <si>
+    <t>TRANSFERENCIA DE FONDOS DEL EXTERIOR SEGUN SOLICITUD</t>
+  </si>
+  <si>
+    <t>EMBAJADAS</t>
+  </si>
+  <si>
+    <t>ORGANISMOS INTERNACIONALES</t>
+  </si>
+  <si>
+    <t>PAGO CHEQUE BRINKS BOLIVIA</t>
+  </si>
+  <si>
+    <t>POR LA VENTA DE DOLARES AMERICANOS</t>
+  </si>
+  <si>
+    <t>INSUMOS Y ADITIVOS</t>
+  </si>
+  <si>
+    <t>PETROBRAS</t>
+  </si>
+  <si>
+    <t>DEPOSITO DE EFECTIVO</t>
+  </si>
+  <si>
+    <t>GASTOS DE FUNCIONAMIENTO</t>
+  </si>
+  <si>
+    <t>AMALGAMATED METAL CORP PLC</t>
+  </si>
+  <si>
+    <t>BIRF</t>
+  </si>
+  <si>
+    <t>GASOLINA BLANCA</t>
+  </si>
+  <si>
+    <t>BOA</t>
+  </si>
+  <si>
+    <t>ETV CON PODER</t>
+  </si>
+  <si>
+    <t>CARTONBOL</t>
+  </si>
+  <si>
+    <t>EASBA</t>
+  </si>
+  <si>
+    <t>CARTA DE CREDITO BCB-IMP</t>
+  </si>
+  <si>
+    <t>YUNTINIC RESOURCES, INC.</t>
+  </si>
+  <si>
+    <t>GLENCORE INTERNATIONAL AG.</t>
+  </si>
+  <si>
+    <t>ELMET S A DE C V (MEXICO)</t>
+  </si>
+  <si>
+    <t>MARCO METALES DE MEXICO</t>
+  </si>
+  <si>
+    <t>ELMET</t>
+  </si>
+  <si>
+    <t>GLP</t>
+  </si>
+  <si>
+    <t>UREA</t>
+  </si>
+  <si>
+    <t>Vinto</t>
+  </si>
+  <si>
+    <t>REMESA DEL EXTERIOR POR EXPORTACI</t>
+  </si>
+  <si>
+    <t>DESEMBOLSO DE PR</t>
+  </si>
+  <si>
+    <t>PAGO DE HABERES</t>
+  </si>
+  <si>
+    <t>COMPENSACION COSTO DE VIDA</t>
+  </si>
+  <si>
+    <t>PAGO POR EL SERVICIO DE TRANSPORTE</t>
+  </si>
+  <si>
+    <t>PAGO A PR</t>
+  </si>
+  <si>
+    <t>Chequear biencito</t>
+  </si>
+  <si>
+    <t>del Chaco</t>
+  </si>
+  <si>
+    <t>FPAH Aportes</t>
+  </si>
+  <si>
+    <t>Banco de Credito</t>
+  </si>
+  <si>
+    <t>Banco Union</t>
+  </si>
+  <si>
+    <t>SEDEM</t>
+  </si>
+  <si>
+    <t>UAGRM</t>
+  </si>
+  <si>
+    <t>EMPRESA NACIONAL DE ELECTRICIDAD</t>
+  </si>
+  <si>
+    <t>MINISTERIO DE RELACIONES EXTERIORES</t>
+  </si>
+  <si>
+    <t>BOLIVIANA DE AVIACION</t>
+  </si>
+  <si>
+    <t>ADMINISTRACION DE SERVICIOS PORTUARIOS BOLIVIA</t>
+  </si>
+  <si>
+    <t>CONSULADO GENERAL DE BOLIVIA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -906,6 +1087,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -928,10 +1122,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2842,8 +3038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2854,27 +3050,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B1" t="s">
         <v>278</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D1" t="s">
+        <v>281</v>
+      </c>
+      <c r="E1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F1" t="s">
         <v>279</v>
-      </c>
-      <c r="C1" t="s">
-        <v>277</v>
-      </c>
-      <c r="D1" t="s">
-        <v>282</v>
-      </c>
-      <c r="E1" t="s">
-        <v>281</v>
-      </c>
-      <c r="F1" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B2">
         <v>404</v>
@@ -2894,7 +3090,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B3">
         <v>404</v>
@@ -2914,7 +3110,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B4">
         <v>404</v>
@@ -2925,16 +3121,10 @@
       <c r="D4" t="s">
         <v>233</v>
       </c>
-      <c r="E4" t="s">
-        <v>271</v>
-      </c>
-      <c r="F4" t="s">
-        <v>271</v>
-      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B5">
         <v>404</v>
@@ -2945,16 +3135,10 @@
       <c r="D5" t="s">
         <v>233</v>
       </c>
-      <c r="E5" t="s">
-        <v>271</v>
-      </c>
-      <c r="F5" t="s">
-        <v>271</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B6">
         <v>404</v>
@@ -2974,7 +3158,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B7">
         <v>404</v>
@@ -2995,7 +3179,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B8">
         <v>404</v>
@@ -3016,7 +3200,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B9">
         <v>412</v>
@@ -3027,16 +3211,10 @@
       <c r="D9" t="s">
         <v>237</v>
       </c>
-      <c r="E9" t="s">
-        <v>271</v>
-      </c>
-      <c r="F9" t="s">
-        <v>271</v>
-      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B10">
         <v>412</v>
@@ -3047,16 +3225,10 @@
       <c r="D10" t="s">
         <v>237</v>
       </c>
-      <c r="E10" t="s">
-        <v>271</v>
-      </c>
-      <c r="F10" t="s">
-        <v>271</v>
-      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B11">
         <v>412</v>
@@ -3077,7 +3249,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B12">
         <v>412</v>
@@ -3088,16 +3260,10 @@
       <c r="D12" t="s">
         <v>239</v>
       </c>
-      <c r="E12" t="s">
-        <v>271</v>
-      </c>
-      <c r="F12" t="s">
-        <v>271</v>
-      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B13">
         <v>412</v>
@@ -3108,16 +3274,10 @@
       <c r="D13" t="s">
         <v>239</v>
       </c>
-      <c r="E13" t="s">
-        <v>271</v>
-      </c>
-      <c r="F13" t="s">
-        <v>271</v>
-      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B14">
         <v>412</v>
@@ -3138,7 +3298,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B15">
         <v>412</v>
@@ -3159,7 +3319,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B16">
         <v>412</v>
@@ -3180,7 +3340,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B17">
         <v>412</v>
@@ -3191,16 +3351,10 @@
       <c r="D17" t="s">
         <v>239</v>
       </c>
-      <c r="E17" t="s">
-        <v>271</v>
-      </c>
-      <c r="F17" t="s">
-        <v>271</v>
-      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B18">
         <v>412</v>
@@ -3211,16 +3365,10 @@
       <c r="D18" t="s">
         <v>239</v>
       </c>
-      <c r="E18" t="s">
-        <v>271</v>
-      </c>
-      <c r="F18" t="s">
-        <v>271</v>
-      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B19">
         <v>403</v>
@@ -3241,7 +3389,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B20">
         <v>403</v>
@@ -3261,7 +3409,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B21">
         <v>403</v>
@@ -3281,7 +3429,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B22">
         <v>403</v>
@@ -3301,7 +3449,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B23">
         <v>403</v>
@@ -3321,7 +3469,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B24">
         <v>403</v>
@@ -3341,7 +3489,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B25">
         <v>403</v>
@@ -3361,7 +3509,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B26">
         <v>403</v>
@@ -3381,7 +3529,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B27">
         <v>403</v>
@@ -3401,7 +3549,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B28">
         <v>403</v>
@@ -3421,7 +3569,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B29">
         <v>403</v>
@@ -3441,7 +3589,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B30">
         <v>403</v>
@@ -3461,7 +3609,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B31">
         <v>403</v>
@@ -3481,7 +3629,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B32">
         <v>403</v>
@@ -3501,7 +3649,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B33">
         <v>403</v>
@@ -3521,7 +3669,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B34">
         <v>403</v>
@@ -3541,7 +3689,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B35">
         <v>403</v>
@@ -3561,7 +3709,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B36">
         <v>403</v>
@@ -3581,7 +3729,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B37">
         <v>403</v>
@@ -3601,7 +3749,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B38">
         <v>403</v>
@@ -3621,7 +3769,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B39">
         <v>403</v>
@@ -3641,7 +3789,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B40">
         <v>403</v>
@@ -3661,7 +3809,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B41">
         <v>403</v>
@@ -3681,7 +3829,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B42">
         <v>403</v>
@@ -3701,7 +3849,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B43">
         <v>403</v>
@@ -3721,7 +3869,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B44">
         <v>403</v>
@@ -3741,7 +3889,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B45">
         <v>403</v>
@@ -3761,7 +3909,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B46">
         <v>403</v>
@@ -3781,7 +3929,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B47">
         <v>403</v>
@@ -3802,7 +3950,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B48">
         <v>405</v>
@@ -3816,13 +3964,10 @@
       <c r="E48" t="s">
         <v>96</v>
       </c>
-      <c r="F48" t="s">
-        <v>271</v>
-      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B49">
         <v>405</v>
@@ -3836,13 +3981,10 @@
       <c r="E49" t="s">
         <v>99</v>
       </c>
-      <c r="F49" t="s">
-        <v>271</v>
-      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B50">
         <v>405</v>
@@ -3851,7 +3993,7 @@
         <v>7329</v>
       </c>
       <c r="D50" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E50" t="s">
         <v>99</v>
@@ -3859,7 +4001,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B51">
         <v>406</v>
@@ -3873,13 +4015,10 @@
       <c r="E51" t="s">
         <v>34</v>
       </c>
-      <c r="F51" t="s">
-        <v>271</v>
-      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B52">
         <v>406</v>
@@ -3893,13 +4032,10 @@
       <c r="E52" t="s">
         <v>34</v>
       </c>
-      <c r="F52" t="s">
-        <v>271</v>
-      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B53">
         <v>406</v>
@@ -3920,7 +4056,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B54">
         <v>414</v>
@@ -3934,13 +4070,10 @@
       <c r="E54" t="s">
         <v>56</v>
       </c>
-      <c r="F54" t="s">
-        <v>271</v>
-      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B55">
         <v>414</v>
@@ -3954,13 +4087,10 @@
       <c r="E55" t="s">
         <v>85</v>
       </c>
-      <c r="F55" t="s">
-        <v>271</v>
-      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B56">
         <v>414</v>
@@ -3974,13 +4104,10 @@
       <c r="E56" t="s">
         <v>85</v>
       </c>
-      <c r="F56" t="s">
-        <v>271</v>
-      </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B57">
         <v>485</v>
@@ -3994,13 +4121,10 @@
       <c r="E57" t="s">
         <v>115</v>
       </c>
-      <c r="F57" t="s">
-        <v>271</v>
-      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B58">
         <v>498</v>
@@ -4014,13 +4138,10 @@
       <c r="E58" t="s">
         <v>135</v>
       </c>
-      <c r="F58" t="s">
-        <v>271</v>
-      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B59">
         <v>499</v>
@@ -4041,7 +4162,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B60">
         <v>499</v>
@@ -4062,7 +4183,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B61">
         <v>606</v>
@@ -4083,7 +4204,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B62">
         <v>606</v>
@@ -4104,7 +4225,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B63">
         <v>828</v>
@@ -4118,13 +4239,10 @@
       <c r="E63" t="s">
         <v>115</v>
       </c>
-      <c r="F63" t="s">
-        <v>271</v>
-      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B64">
         <v>201</v>
@@ -4138,13 +4256,10 @@
       <c r="E64" t="s">
         <v>115</v>
       </c>
-      <c r="F64" t="s">
-        <v>271</v>
-      </c>
     </row>
     <row r="65" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B65" s="1">
         <v>498</v>
@@ -4153,18 +4268,14 @@
         <v>6818</v>
       </c>
       <c r="D65" t="s">
-        <v>283</v>
-      </c>
-      <c r="E65" t="s">
-        <v>271</v>
-      </c>
-      <c r="F65" t="s">
-        <v>271</v>
-      </c>
+        <v>282</v>
+      </c>
+      <c r="E65"/>
+      <c r="F65"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B66">
         <v>25</v>
@@ -4173,18 +4284,18 @@
         <v>166</v>
       </c>
       <c r="D66" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E66" t="s">
         <v>103</v>
       </c>
       <c r="F66" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B67">
         <v>25</v>
@@ -4193,18 +4304,18 @@
         <v>9999</v>
       </c>
       <c r="D67" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E67" t="s">
         <v>31</v>
       </c>
       <c r="F67" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B68">
         <v>828</v>
@@ -4213,18 +4324,15 @@
         <v>3500</v>
       </c>
       <c r="D68" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E68" t="s">
         <v>49</v>
       </c>
-      <c r="F68" t="s">
-        <v>271</v>
-      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B69">
         <v>10</v>
@@ -4233,16 +4341,692 @@
         <v>6535</v>
       </c>
       <c r="D69" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E69" t="s">
         <v>115</v>
       </c>
       <c r="F69" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B82"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>285</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>288</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>289</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>308</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>290</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>291</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>292</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>299</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>327</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>300</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>293</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>309</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>301</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>302</v>
+      </c>
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>328</v>
+      </c>
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>303</v>
+      </c>
+      <c r="B20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>304</v>
+      </c>
+      <c r="B21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>296</v>
+      </c>
+      <c r="B22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>297</v>
+      </c>
+      <c r="B23" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>329</v>
+      </c>
+      <c r="B24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>330</v>
+      </c>
+      <c r="B25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>298</v>
+      </c>
+      <c r="B26" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>331</v>
+      </c>
+      <c r="B27" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>310</v>
+      </c>
+      <c r="B28" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>305</v>
+      </c>
+      <c r="B30" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>294</v>
+      </c>
+      <c r="B31" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>295</v>
+      </c>
+      <c r="B32" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>311</v>
+      </c>
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>306</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>312</v>
+      </c>
+      <c r="B35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>313</v>
+      </c>
+      <c r="B36" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>314</v>
+      </c>
+      <c r="B37" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>307</v>
+      </c>
+      <c r="B38" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>315</v>
+      </c>
+      <c r="B39" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>316</v>
+      </c>
+      <c r="B40" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>317</v>
+      </c>
+      <c r="B41" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>318</v>
+      </c>
+      <c r="B42" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>319</v>
+      </c>
+      <c r="B43" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>320</v>
+      </c>
+      <c r="B44" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>321</v>
+      </c>
+      <c r="B45" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>323</v>
+      </c>
+      <c r="B46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>322</v>
+      </c>
+      <c r="B47" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>241</v>
+      </c>
+      <c r="B48" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>242</v>
+      </c>
+      <c r="B49" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>336</v>
+      </c>
+      <c r="B50" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>243</v>
+      </c>
+      <c r="B51" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>244</v>
+      </c>
+      <c r="B52" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>337</v>
+      </c>
+      <c r="B53" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>245</v>
+      </c>
+      <c r="B54" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>246</v>
+      </c>
+      <c r="B55" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>247</v>
+      </c>
+      <c r="B56" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>248</v>
+      </c>
+      <c r="B57" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>249</v>
+      </c>
+      <c r="B58" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>250</v>
+      </c>
+      <c r="B59" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>251</v>
+      </c>
+      <c r="B60" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>252</v>
+      </c>
+      <c r="B61" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>253</v>
+      </c>
+      <c r="B62" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>254</v>
+      </c>
+      <c r="B63" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>324</v>
+      </c>
+      <c r="B64" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>325</v>
+      </c>
+      <c r="B65" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>334</v>
+      </c>
+      <c r="B66" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>326</v>
+      </c>
+      <c r="B67" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>238</v>
+      </c>
+      <c r="B68" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>240</v>
+      </c>
+      <c r="B69" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>263</v>
+      </c>
+      <c r="B70" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>270</v>
+      </c>
+      <c r="B71" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>255</v>
+      </c>
+      <c r="B72" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>257</v>
+      </c>
+      <c r="B73" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>260</v>
+      </c>
+      <c r="B74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>335</v>
+      </c>
+      <c r="B75" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>338</v>
+      </c>
+      <c r="B76" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="B77" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>340</v>
+      </c>
+      <c r="B78" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>341</v>
+      </c>
+      <c r="B79" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>342</v>
+      </c>
+      <c r="B80" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>343</v>
+      </c>
+      <c r="B81" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>344</v>
+      </c>
+      <c r="B82" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ya hicimos la presentación faltan cosas
</commit_message>
<xml_diff>
--- a/data/parametros.xlsx
+++ b/data/parametros.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="350">
   <si>
     <t>Nivel 2</t>
   </si>
@@ -1061,6 +1061,21 @@
   </si>
   <si>
     <t>CONSULADO GENERAL DE BOLIVIA</t>
+  </si>
+  <si>
+    <t>PETROPERU</t>
+  </si>
+  <si>
+    <t>VITOL</t>
+  </si>
+  <si>
+    <t>CONSULADO DE BOLIVIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMBAJADA DE BOLIVIA </t>
+  </si>
+  <si>
+    <t>LA PRIMERA</t>
   </si>
 </sst>
 </file>
@@ -4357,10 +4372,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B82"/>
+  <dimension ref="A1:B87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5025,6 +5040,46 @@
         <v>34</v>
       </c>
     </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>345</v>
+      </c>
+      <c r="B83" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>346</v>
+      </c>
+      <c r="B84" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>347</v>
+      </c>
+      <c r="B85" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>348</v>
+      </c>
+      <c r="B86" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>349</v>
+      </c>
+      <c r="B87" t="s">
+        <v>333</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>